<commit_message>
Add all entities db
</commit_message>
<xml_diff>
--- a/db/Materia.xlsx
+++ b/db/Materia.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Documents\Posgrado\Proyecto Titulacion\db\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PosGrado\Proyecto Titulacion\Timetabling\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D070976A-6584-4129-B5F1-CF18E6FE8729}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74A70D73-3D96-4F99-AF78-C01909FE9452}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{73FF22F9-0A89-43F3-8B4B-2BA89E274F19}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{73FF22F9-0A89-43F3-8B4B-2BA89E274F19}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -27,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -44,9 +42,6 @@
     <t>nombre_materia</t>
   </si>
   <si>
-    <t>dia_fijo</t>
-  </si>
-  <si>
     <t>horas_semanales_tipicas</t>
   </si>
   <si>
@@ -60,13 +55,16 @@
   </si>
   <si>
     <t>Ritmica</t>
+  </si>
+  <si>
+    <t>Tipo de materia</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -434,16 +432,17 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
   <cols>
-    <col min="2" max="2" width="14.33203125" customWidth="1"/>
-    <col min="4" max="4" width="21.88671875" customWidth="1"/>
+    <col min="2" max="2" width="14.375" customWidth="1"/>
+    <col min="3" max="3" width="14" customWidth="1"/>
+    <col min="4" max="4" width="21.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -451,30 +450,30 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+    </row>
+    <row r="2" spans="1:4">
+      <c r="B2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B2" t="s">
+    <row r="3" spans="1:4">
+      <c r="B3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B3" t="s">
+    <row r="4" spans="1:4">
+      <c r="B4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
+    <row r="5" spans="1:4">
+      <c r="B5" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>